<commit_message>
My Project details ONLINE BANKING SYSTEM
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="76">
   <si>
     <t>beneficiary</t>
   </si>
@@ -278,6 +278,12 @@
   <si>
     <t>Incorrect OTP
 Please try again</t>
+  </si>
+  <si>
+    <t>Application submitted successfully
+Application number : 162434932
+Please visit bank with application number for account approval
+Hint: From staff login, approve application</t>
   </si>
 </sst>
 </file>
@@ -851,9 +857,9 @@
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="F31" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
@@ -957,7 +963,7 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>